<commit_message>
fix VND data output
</commit_message>
<xml_diff>
--- a/file/stock-output/interesting-stock/SET/SET-interesting-company-info.xlsx
+++ b/file/stock-output/interesting-stock/SET/SET-interesting-company-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekala\PycharmProjects\SET-stock-analysis\file\stock-output\interesting-stock\SET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960747BD-0F87-40AD-9183-27AFC4DAB91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B39DBFA-E355-4EEA-88E9-77C041C76895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5640" yWindow="2280" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2040,12 +2040,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A143" sqref="A143"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="43.7109375" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>